<commit_message>
Added functionality to view invoice with corresponding lines
</commit_message>
<xml_diff>
--- a/db_tools/acctg_db5/acctg_export5.xlsx
+++ b/db_tools/acctg_db5/acctg_export5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingPython\thanos_app\db_tools\acctg_db5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405BD60A-205D-4FEC-A32A-A089FD0E9A98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943627CE-24F5-4904-9DC7-4A8DE1374590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="1440" windowWidth="21600" windowHeight="11235" firstSheet="18" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2824" uniqueCount="1211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3002" uniqueCount="1211">
   <si>
     <t>id</t>
   </si>
@@ -4058,15 +4058,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4097,8 +4097,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4129,8 +4132,11 @@
       <c r="J2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4161,8 +4167,11 @@
       <c r="J3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4193,8 +4202,11 @@
       <c r="J4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4225,8 +4237,11 @@
       <c r="J5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4256,6 +4271,9 @@
       </c>
       <c r="J6" t="s">
         <v>50</v>
+      </c>
+      <c r="K6" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4265,13 +4283,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4281,8 +4301,11 @@
       <c r="C1" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4292,8 +4315,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4303,8 +4329,11 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4314,8 +4343,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4325,8 +4357,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4336,8 +4371,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4346,6 +4384,9 @@
       </c>
       <c r="C7">
         <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4530,7 +4571,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -8768,8 +8811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13388,13 +13431,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13416,8 +13461,11 @@
       <c r="G1" s="1" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13439,8 +13487,11 @@
       <c r="G2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -13462,8 +13513,11 @@
       <c r="G3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -13485,8 +13539,11 @@
       <c r="G4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -13508,8 +13565,11 @@
       <c r="G5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -13531,8 +13591,11 @@
       <c r="G6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -13554,8 +13617,11 @@
       <c r="G7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13577,8 +13643,11 @@
       <c r="G8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -13600,8 +13669,11 @@
       <c r="G9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -13623,8 +13695,11 @@
       <c r="G10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -13646,8 +13721,11 @@
       <c r="G11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -13669,8 +13747,11 @@
       <c r="G12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -13692,8 +13773,11 @@
       <c r="G13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -13715,8 +13799,11 @@
       <c r="G14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -13738,8 +13825,11 @@
       <c r="G15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -13761,8 +13851,11 @@
       <c r="G16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -13784,8 +13877,11 @@
       <c r="G17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -13807,8 +13903,11 @@
       <c r="G18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -13830,8 +13929,11 @@
       <c r="G19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -13853,8 +13955,11 @@
       <c r="G20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -13876,8 +13981,11 @@
       <c r="G21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -13899,8 +14007,11 @@
       <c r="G22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -13922,8 +14033,11 @@
       <c r="G23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -13945,8 +14059,11 @@
       <c r="G24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -13968,8 +14085,11 @@
       <c r="G25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -13991,8 +14111,11 @@
       <c r="G26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -14014,8 +14137,11 @@
       <c r="G27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -14037,8 +14163,11 @@
       <c r="G28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -14060,8 +14189,11 @@
       <c r="G29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -14083,8 +14215,11 @@
       <c r="G30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -14106,8 +14241,11 @@
       <c r="G31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -14129,8 +14267,11 @@
       <c r="G32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -14152,8 +14293,11 @@
       <c r="G33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -14175,8 +14319,11 @@
       <c r="G34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -14198,8 +14345,11 @@
       <c r="G35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -14221,8 +14371,11 @@
       <c r="G36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -14244,8 +14397,11 @@
       <c r="G37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -14267,8 +14423,11 @@
       <c r="G38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -14290,8 +14449,11 @@
       <c r="G39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -14313,8 +14475,11 @@
       <c r="G40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -14336,8 +14501,11 @@
       <c r="G41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -14359,8 +14527,11 @@
       <c r="G42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -14382,8 +14553,11 @@
       <c r="G43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -14405,8 +14579,11 @@
       <c r="G44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -14428,8 +14605,11 @@
       <c r="G45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -14451,8 +14631,11 @@
       <c r="G46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -14474,8 +14657,11 @@
       <c r="G47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H47" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -14497,8 +14683,11 @@
       <c r="G48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -14520,8 +14709,11 @@
       <c r="G49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H49" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -14543,8 +14735,11 @@
       <c r="G50">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -14566,8 +14761,11 @@
       <c r="G51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -14589,8 +14787,11 @@
       <c r="G52">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -14612,8 +14813,11 @@
       <c r="G53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -14635,8 +14839,11 @@
       <c r="G54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H54" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -14658,8 +14865,11 @@
       <c r="G55">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H55" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -14681,8 +14891,11 @@
       <c r="G56">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -14704,8 +14917,11 @@
       <c r="G57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -14726,6 +14942,9 @@
       </c>
       <c r="G58">
         <v>5</v>
+      </c>
+      <c r="H58" t="s">
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -19729,7 +19948,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -19806,13 +20027,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -19834,8 +20057,11 @@
       <c r="G1" s="1" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -19857,8 +20083,11 @@
       <c r="G2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -19880,8 +20109,11 @@
       <c r="G3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -19903,8 +20135,11 @@
       <c r="G4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -19926,8 +20161,11 @@
       <c r="G5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -19949,8 +20187,11 @@
       <c r="G6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -19972,8 +20213,11 @@
       <c r="G7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -19995,8 +20239,11 @@
       <c r="G8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -20018,8 +20265,11 @@
       <c r="G9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -20041,8 +20291,11 @@
       <c r="G10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -20064,8 +20317,11 @@
       <c r="G11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -20087,8 +20343,11 @@
       <c r="G12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -20110,8 +20369,11 @@
       <c r="G13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -20133,8 +20395,11 @@
       <c r="G14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -20156,8 +20421,11 @@
       <c r="G15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -20179,8 +20447,11 @@
       <c r="G16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -20202,8 +20473,11 @@
       <c r="G17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -20225,8 +20499,11 @@
       <c r="G18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -20248,8 +20525,11 @@
       <c r="G19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -20271,8 +20551,11 @@
       <c r="G20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -20294,8 +20577,11 @@
       <c r="G21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -20317,8 +20603,11 @@
       <c r="G22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -20340,8 +20629,11 @@
       <c r="G23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -20363,8 +20655,11 @@
       <c r="G24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -20386,8 +20681,11 @@
       <c r="G25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -20409,8 +20707,11 @@
       <c r="G26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -20432,8 +20733,11 @@
       <c r="G27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -20455,8 +20759,11 @@
       <c r="G28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -20478,8 +20785,11 @@
       <c r="G29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -20501,8 +20811,11 @@
       <c r="G30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -20524,8 +20837,11 @@
       <c r="G31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -20547,8 +20863,11 @@
       <c r="G32">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H32" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -20570,8 +20889,11 @@
       <c r="G33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -20593,8 +20915,11 @@
       <c r="G34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -20616,8 +20941,11 @@
       <c r="G35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -20639,8 +20967,11 @@
       <c r="G36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -20662,8 +20993,11 @@
       <c r="G37">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -20685,8 +21019,11 @@
       <c r="G38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -20708,8 +21045,11 @@
       <c r="G39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -20731,8 +21071,11 @@
       <c r="G40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -20754,8 +21097,11 @@
       <c r="G41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -20777,8 +21123,11 @@
       <c r="G42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -20800,8 +21149,11 @@
       <c r="G43">
         <v>5</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -20823,8 +21175,11 @@
       <c r="G44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -20846,8 +21201,11 @@
       <c r="G45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -20869,8 +21227,11 @@
       <c r="G46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -20892,8 +21253,11 @@
       <c r="G47">
         <v>5</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H47" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -20915,8 +21279,11 @@
       <c r="G48">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H48" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -20938,8 +21305,11 @@
       <c r="G49">
         <v>5</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H49" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -20961,8 +21331,11 @@
       <c r="G50">
         <v>5</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H50" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -20984,8 +21357,11 @@
       <c r="G51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H51" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -21007,8 +21383,11 @@
       <c r="G52">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H52" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -21030,8 +21409,11 @@
       <c r="G53">
         <v>5</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H53" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -21053,8 +21435,11 @@
       <c r="G54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H54" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -21076,8 +21461,11 @@
       <c r="G55">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H55" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -21099,8 +21487,11 @@
       <c r="G56">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H56" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -21122,8 +21513,11 @@
       <c r="G57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H57" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -21144,6 +21538,9 @@
       </c>
       <c r="G58">
         <v>5</v>
+      </c>
+      <c r="H58" t="s">
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -21153,10 +21550,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="M37" sqref="M2:M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -21174,7 +21571,7 @@
     <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -21211,8 +21608,11 @@
       <c r="L1" s="1" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -21243,8 +21643,11 @@
       <c r="L2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -21275,8 +21678,11 @@
       <c r="L3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -21310,8 +21716,11 @@
       <c r="L4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -21345,8 +21754,11 @@
       <c r="L5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -21377,8 +21789,11 @@
       <c r="L6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -21409,8 +21824,11 @@
       <c r="L7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -21444,8 +21862,11 @@
       <c r="L8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -21476,8 +21897,11 @@
       <c r="L9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -21508,8 +21932,11 @@
       <c r="L10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -21540,8 +21967,11 @@
       <c r="L11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -21575,8 +22005,11 @@
       <c r="L12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -21607,8 +22040,11 @@
       <c r="L13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -21639,8 +22075,11 @@
       <c r="L14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -21674,8 +22113,11 @@
       <c r="L15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -21706,8 +22148,11 @@
       <c r="L16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -21738,8 +22183,11 @@
       <c r="L17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -21770,8 +22218,11 @@
       <c r="L18">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -21802,8 +22253,11 @@
       <c r="L19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -21837,8 +22291,11 @@
       <c r="L20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -21869,8 +22326,11 @@
       <c r="L21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -21901,8 +22361,11 @@
       <c r="L22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -21933,8 +22396,11 @@
       <c r="L23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -21965,8 +22431,11 @@
       <c r="L24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -22000,8 +22469,11 @@
       <c r="L25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -22032,8 +22504,11 @@
       <c r="L26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -22064,8 +22539,11 @@
       <c r="L27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -22096,8 +22574,11 @@
       <c r="L28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -22131,8 +22612,11 @@
       <c r="L29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -22163,8 +22647,11 @@
       <c r="L30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -22195,8 +22682,11 @@
       <c r="L31">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -22227,8 +22717,11 @@
       <c r="L32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M32" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -22259,8 +22752,11 @@
       <c r="L33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -22294,8 +22790,11 @@
       <c r="L34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -22326,8 +22825,11 @@
       <c r="L35">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -22358,8 +22860,11 @@
       <c r="L36">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -22389,6 +22894,9 @@
       </c>
       <c r="L37">
         <v>6</v>
+      </c>
+      <c r="M37" t="s">
+        <v>544</v>
       </c>
     </row>
   </sheetData>
@@ -23441,7 +23949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:K151"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -27390,7 +27898,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28777,8 +29285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O1:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29185,7 +29693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29627E5B-8817-45BF-AA5B-EB0E6F6034B9}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -29991,7 +30499,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -30082,13 +30592,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -30104,8 +30616,11 @@
       <c r="E1" s="1" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -30121,8 +30636,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -30138,8 +30656,11 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -30155,8 +30676,11 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -30172,8 +30696,11 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -30188,6 +30715,9 @@
       </c>
       <c r="E6">
         <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -30197,13 +30727,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -30219,8 +30751,11 @@
       <c r="E1" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -30236,8 +30771,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -30253,8 +30791,11 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -30270,8 +30811,11 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -30287,8 +30831,11 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -30303,6 +30850,9 @@
       </c>
       <c r="E6">
         <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added db tools to use mysql instead
</commit_message>
<xml_diff>
--- a/db_tools/acctg_db5/acctg_export5.xlsx
+++ b/db_tools/acctg_db5/acctg_export5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgrammingPython\thanos_app\db_tools\acctg_db5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943627CE-24F5-4904-9DC7-4A8DE1374590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C0C7B5-8F8F-49D9-91CB-5125586ECEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="1440" windowWidth="21600" windowHeight="11235" firstSheet="18" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="18" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="1" r:id="rId1"/>
@@ -22909,7 +22909,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -23192,7 +23194,7 @@
         <v>700</v>
       </c>
       <c r="H9">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="I9">
         <v>2100</v>
@@ -23949,7 +23951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:K151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>